<commit_message>
moved due to new folder structure
</commit_message>
<xml_diff>
--- a/ESA/ESA_Alc_Share_240221.xlsx
+++ b/ESA/ESA_Alc_Share_240221.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\50-Projekte\483-Bund ESA\_Publ\2024_Alc share of total consumption\Tables\Sent_240221\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annas\Documents\ISD\alc_revenue_distribution\ESA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABA82FD-A33F-40BA-AE59-AB571257DB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB7119B-B7A7-4B52-A984-A7FE0A1DB030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{ABF30B17-BF89-4028-B4A7-10D8277C2E13}"/>
+    <workbookView xWindow="33240" yWindow="1455" windowWidth="21600" windowHeight="15315" activeTab="2" xr2:uid="{ABF30B17-BF89-4028-B4A7-10D8277C2E13}"/>
   </bookViews>
   <sheets>
     <sheet name="Variablen_Übersicht" sheetId="3" r:id="rId1"/>
@@ -289,9 +289,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="172" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -357,10 +357,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -380,9 +380,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -420,7 +420,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -526,7 +526,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -668,7 +668,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -678,24 +678,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFA0A3FA-2FE0-4CCA-A85D-C0810A7323AA}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="5"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -706,7 +706,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -723,7 +723,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -740,7 +740,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -757,7 +757,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -774,7 +774,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -782,7 +782,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -790,7 +790,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -798,7 +798,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -806,7 +806,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -814,7 +814,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -822,7 +822,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -830,7 +830,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -838,7 +838,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -846,7 +846,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -854,7 +854,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>52</v>
       </c>
@@ -862,7 +862,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -870,7 +870,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -878,7 +878,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -886,7 +886,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -894,13 +894,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -908,7 +908,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -916,7 +916,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -924,7 +924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -932,7 +932,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -940,7 +940,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -948,7 +948,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -956,7 +956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -964,7 +964,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -972,7 +972,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -980,7 +980,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -988,7 +988,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -996,7 +996,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -1043,30 +1043,30 @@
   <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J64" sqref="J64"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4476,8 +4476,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:20">
-      <c r="I58" s="6"/>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="I58" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4488,18 +4488,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3730A246-C5F4-48BB-A204-68BB141E0D55}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>5.3192530010692884</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>3.7796929702010704</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>2.965981250786792</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>4.3569512073499457</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>4.2806152185423354</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>6.6850742837209554</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>3.8777661550648497</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>2.5091183779351449</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>5.3867043585495642</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>4.5104202116457044</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>6.7972090575781348</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>9.1123058963050703</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>4.5923371051267097</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>4.6321217950205202</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>11.259690343049778</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>4.1623563764493614</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>3.326935829571843</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>

</xml_diff>